<commit_message>
added assertions to 30 espn test cases
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA4381A-9F1E-4D87-A791-23710DB2202D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39037C-A155-4400-B84D-FC22037C09D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
   <si>
     <t>City Name</t>
   </si>
@@ -221,10 +221,97 @@
     <t>Spurs</t>
   </si>
   <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Atlanta Hawks</t>
+  </si>
+  <si>
     <t>Boston Celtics</t>
   </si>
   <si>
     <t>Brooklyn Nets</t>
+  </si>
+  <si>
+    <t>Charlotte Hornets</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Detroit Pistons</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Golden State Warriors</t>
+  </si>
+  <si>
+    <t>Houston Rockets</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>LA Clippers</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers</t>
+  </si>
+  <si>
+    <t>Memphis Grizzlies</t>
+  </si>
+  <si>
+    <t>Miami Heat</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks</t>
+  </si>
+  <si>
+    <t>Minnesota Timberwolves</t>
+  </si>
+  <si>
+    <t>New Orleans Pelicans</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>Philadelphia 76ers</t>
+  </si>
+  <si>
+    <t>Phoenix Suns</t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers</t>
+  </si>
+  <si>
+    <t>Sacramento Kings</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs</t>
+  </si>
+  <si>
+    <t>Toronto Raptors</t>
+  </si>
+  <si>
+    <t>Utah Jazz</t>
+  </si>
+  <si>
+    <t>Washington Wizards</t>
   </si>
 </sst>
 </file>
@@ -580,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AF868F-1619-4058-BC1A-5F3E5C88CA24}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,245 +687,248 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -846,113 +936,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA23FD94-FD19-4660-99A3-376865924FBE}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>44</v>
@@ -960,79 +1053,79 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>54</v>
@@ -1040,50 +1133,66 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored espn module (still needs to be cleaned and organized some more)
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39037C-A155-4400-B84D-FC22037C09D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018069D0-D755-4C03-91F2-31E72ACEA8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
-    <sheet name="nbaTeams" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>City Name</t>
   </si>
@@ -312,14 +312,25 @@
   </si>
   <si>
     <t>Washington Wizards</t>
+  </si>
+  <si>
+    <t>NBA Teams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -347,10 +358,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,11 +676,216 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA23FD94-FD19-4660-99A3-376865924FBE}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AF868F-1619-4058-BC1A-5F3E5C88CA24}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection sqref="A1:B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,10 +895,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -932,270 +1149,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA23FD94-FD19-4660-99A3-376865924FBE}">
-  <dimension ref="A1:B31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
documenting espn test cases
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data.xlsx
+++ b/com.espn/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018069D0-D755-4C03-91F2-31E72ACEA8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6149ECCB-0FE9-48AD-80A1-D5AEAC40F653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
+    <sheet name="nbaCityNameTeamName" sheetId="1" r:id="rId2"/>
+    <sheet name="nbaPage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>City Name</t>
   </si>
@@ -315,6 +316,12 @@
   </si>
   <si>
     <t>NBA Teams</t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>Assertions</t>
   </si>
 </sst>
 </file>
@@ -358,11 +365,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA23FD94-FD19-4660-99A3-376865924FBE}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,6 +882,9 @@
       </c>
       <c r="B31" s="1"/>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -884,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AF868F-1619-4058-BC1A-5F3E5C88CA24}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1149,4 +1160,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF61E29-BE99-4C4C-9C35-39643D902B90}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>